<commit_message>
Created figures with english text
</commit_message>
<xml_diff>
--- a/Data/Bees_Vestlandet_SiljeOgSara.xlsx
+++ b/Data/Bees_Vestlandet_SiljeOgSara.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Aktive\DMS\6400_bg\52319_GreenRoad\STIPENDIAT AP3.1 POLLINERING\R\PollinationApples\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AD0F1C-3136-44E2-812F-893B2FF4DD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FED0B-0E79-4437-9B02-25FE5EFBAA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{80059B07-CD8C-4FAD-AA69-ACB8DCA40CA6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="98">
   <si>
     <t>Location</t>
   </si>
@@ -318,6 +318,21 @@
   </si>
   <si>
     <t>Norsk_gruppe</t>
+  </si>
+  <si>
+    <t>English_gruppe</t>
+  </si>
+  <si>
+    <t>Wild bee</t>
+  </si>
+  <si>
+    <t>Hoverfly</t>
+  </si>
+  <si>
+    <t>Honeybee</t>
+  </si>
+  <si>
+    <t>Bumble bee</t>
   </si>
 </sst>
 </file>
@@ -731,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F217761-C46D-4553-9B08-6E524775D494}">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="D242" sqref="D242"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,10 +757,10 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="32.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.453125" style="5" customWidth="1"/>
-    <col min="4" max="5" width="18" style="5" customWidth="1"/>
+    <col min="4" max="6" width="18" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -761,8 +776,11 @@
       <c r="E1" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -778,8 +796,11 @@
       <c r="E2" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -795,8 +816,11 @@
       <c r="E3" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -812,8 +836,11 @@
       <c r="E4" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -829,8 +856,11 @@
       <c r="E5" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -846,8 +876,11 @@
       <c r="E6" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -863,8 +896,11 @@
       <c r="E7" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -880,8 +916,11 @@
       <c r="E8" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -897,8 +936,11 @@
       <c r="E9" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -914,8 +956,11 @@
       <c r="E10" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -931,8 +976,11 @@
       <c r="E11" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -948,8 +996,11 @@
       <c r="E12" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
@@ -965,8 +1016,11 @@
       <c r="E13" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
@@ -982,8 +1036,11 @@
       <c r="E14" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
@@ -999,8 +1056,11 @@
       <c r="E15" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1016,8 +1076,11 @@
       <c r="E16" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1033,8 +1096,11 @@
       <c r="E17" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1050,8 +1116,11 @@
       <c r="E18" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1067,8 +1136,11 @@
       <c r="E19" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1084,8 +1156,11 @@
       <c r="E20" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1101,8 +1176,11 @@
       <c r="E21" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1118,8 +1196,11 @@
       <c r="E22" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1135,8 +1216,11 @@
       <c r="E23" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>71</v>
       </c>
@@ -1152,8 +1236,11 @@
       <c r="E24" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>71</v>
       </c>
@@ -1169,8 +1256,11 @@
       <c r="E25" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1186,8 +1276,11 @@
       <c r="E26" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1203,8 +1296,11 @@
       <c r="E27" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -1220,8 +1316,11 @@
       <c r="E28" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
@@ -1237,8 +1336,11 @@
       <c r="E29" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1254,8 +1356,11 @@
       <c r="E30" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1271,8 +1376,11 @@
       <c r="E31" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1288,8 +1396,11 @@
       <c r="E32" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -1305,8 +1416,11 @@
       <c r="E33" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1322,8 +1436,11 @@
       <c r="E34" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1339,8 +1456,11 @@
       <c r="E35" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
@@ -1356,8 +1476,11 @@
       <c r="E36" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
@@ -1373,8 +1496,11 @@
       <c r="E37" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
@@ -1390,8 +1516,11 @@
       <c r="E38" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -1407,8 +1536,11 @@
       <c r="E39" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -1424,8 +1556,11 @@
       <c r="E40" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
@@ -1441,8 +1576,11 @@
       <c r="E41" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>1</v>
       </c>
@@ -1458,8 +1596,11 @@
       <c r="E42" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
@@ -1475,8 +1616,11 @@
       <c r="E43" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -1492,8 +1636,11 @@
       <c r="E44" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
@@ -1509,8 +1656,11 @@
       <c r="E45" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
@@ -1526,8 +1676,11 @@
       <c r="E46" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
@@ -1543,8 +1696,11 @@
       <c r="E47" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -1560,8 +1716,11 @@
       <c r="E48" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
@@ -1577,8 +1736,11 @@
       <c r="E49" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
@@ -1594,8 +1756,11 @@
       <c r="E50" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>71</v>
       </c>
@@ -1611,8 +1776,11 @@
       <c r="E51" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>71</v>
       </c>
@@ -1628,8 +1796,11 @@
       <c r="E52" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>1</v>
       </c>
@@ -1645,8 +1816,11 @@
       <c r="E53" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>1</v>
       </c>
@@ -1662,8 +1836,11 @@
       <c r="E54" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
@@ -1679,8 +1856,11 @@
       <c r="E55" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>13</v>
       </c>
@@ -1696,8 +1876,11 @@
       <c r="E56" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>13</v>
       </c>
@@ -1713,8 +1896,11 @@
       <c r="E57" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>13</v>
       </c>
@@ -1730,8 +1916,11 @@
       <c r="E58" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>1</v>
       </c>
@@ -1747,8 +1936,11 @@
       <c r="E59" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>1</v>
       </c>
@@ -1764,8 +1956,11 @@
       <c r="E60" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>1</v>
       </c>
@@ -1781,8 +1976,11 @@
       <c r="E61" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>1</v>
       </c>
@@ -1798,8 +1996,11 @@
       <c r="E62" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -1815,8 +2016,11 @@
       <c r="E63" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>1</v>
       </c>
@@ -1832,8 +2036,11 @@
       <c r="E64" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>71</v>
       </c>
@@ -1849,8 +2056,11 @@
       <c r="E65" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
@@ -1866,8 +2076,11 @@
       <c r="E66" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>13</v>
       </c>
@@ -1883,8 +2096,11 @@
       <c r="E67" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>71</v>
       </c>
@@ -1900,8 +2116,11 @@
       <c r="E68" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>1</v>
       </c>
@@ -1917,8 +2136,11 @@
       <c r="E69" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>71</v>
       </c>
@@ -1934,8 +2156,11 @@
       <c r="E70" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>13</v>
       </c>
@@ -1951,8 +2176,11 @@
       <c r="E71" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>1</v>
       </c>
@@ -1968,8 +2196,11 @@
       <c r="E72" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>13</v>
       </c>
@@ -1985,8 +2216,11 @@
       <c r="E73" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>1</v>
       </c>
@@ -2002,8 +2236,11 @@
       <c r="E74" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>13</v>
       </c>
@@ -2019,8 +2256,11 @@
       <c r="E75" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>1</v>
       </c>
@@ -2036,8 +2276,11 @@
       <c r="E76" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>1</v>
       </c>
@@ -2053,8 +2296,11 @@
       <c r="E77" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>1</v>
       </c>
@@ -2070,8 +2316,11 @@
       <c r="E78" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>1</v>
       </c>
@@ -2087,8 +2336,11 @@
       <c r="E79" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>1</v>
       </c>
@@ -2104,8 +2356,11 @@
       <c r="E80" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
@@ -2121,8 +2376,11 @@
       <c r="E81" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>1</v>
       </c>
@@ -2138,8 +2396,11 @@
       <c r="E82" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>1</v>
       </c>
@@ -2155,8 +2416,11 @@
       <c r="E83" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>1</v>
       </c>
@@ -2172,8 +2436,11 @@
       <c r="E84" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>1</v>
       </c>
@@ -2189,8 +2456,11 @@
       <c r="E85" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>1</v>
       </c>
@@ -2206,8 +2476,11 @@
       <c r="E86" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>1</v>
       </c>
@@ -2223,8 +2496,11 @@
       <c r="E87" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>1</v>
       </c>
@@ -2240,8 +2516,11 @@
       <c r="E88" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>1</v>
       </c>
@@ -2257,8 +2536,11 @@
       <c r="E89" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>1</v>
       </c>
@@ -2274,8 +2556,11 @@
       <c r="E90" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F90" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>1</v>
       </c>
@@ -2291,8 +2576,11 @@
       <c r="E91" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F91" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>1</v>
       </c>
@@ -2308,8 +2596,11 @@
       <c r="E92" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F92" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>1</v>
       </c>
@@ -2325,8 +2616,11 @@
       <c r="E93" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F93" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>71</v>
       </c>
@@ -2342,8 +2636,11 @@
       <c r="E94" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>1</v>
       </c>
@@ -2359,8 +2656,11 @@
       <c r="E95" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F95" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>1</v>
       </c>
@@ -2376,8 +2676,11 @@
       <c r="E96" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F96" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>1</v>
       </c>
@@ -2393,8 +2696,11 @@
       <c r="E97" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F97" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>1</v>
       </c>
@@ -2410,8 +2716,11 @@
       <c r="E98" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F98" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>1</v>
       </c>
@@ -2427,8 +2736,11 @@
       <c r="E99" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F99" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>1</v>
       </c>
@@ -2444,8 +2756,11 @@
       <c r="E100" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>1</v>
       </c>
@@ -2461,8 +2776,11 @@
       <c r="E101" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F101" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>1</v>
       </c>
@@ -2478,8 +2796,11 @@
       <c r="E102" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F102" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>1</v>
       </c>
@@ -2495,8 +2816,11 @@
       <c r="E103" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F103" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>1</v>
       </c>
@@ -2512,8 +2836,11 @@
       <c r="E104" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F104" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>1</v>
       </c>
@@ -2529,8 +2856,11 @@
       <c r="E105" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F105" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>1</v>
       </c>
@@ -2546,8 +2876,11 @@
       <c r="E106" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F106" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>1</v>
       </c>
@@ -2563,8 +2896,11 @@
       <c r="E107" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F107" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>1</v>
       </c>
@@ -2580,8 +2916,11 @@
       <c r="E108" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F108" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>1</v>
       </c>
@@ -2597,8 +2936,11 @@
       <c r="E109" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F109" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>1</v>
       </c>
@@ -2614,8 +2956,11 @@
       <c r="E110" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F110" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>1</v>
       </c>
@@ -2631,8 +2976,11 @@
       <c r="E111" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F111" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>1</v>
       </c>
@@ -2648,8 +2996,11 @@
       <c r="E112" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F112" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>1</v>
       </c>
@@ -2665,8 +3016,11 @@
       <c r="E113" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F113" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>1</v>
       </c>
@@ -2682,8 +3036,11 @@
       <c r="E114" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F114" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>1</v>
       </c>
@@ -2699,8 +3056,11 @@
       <c r="E115" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F115" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>1</v>
       </c>
@@ -2716,8 +3076,11 @@
       <c r="E116" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F116" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
@@ -2733,8 +3096,11 @@
       <c r="E117" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F117" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>1</v>
       </c>
@@ -2750,8 +3116,11 @@
       <c r="E118" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F118" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>1</v>
       </c>
@@ -2767,8 +3136,11 @@
       <c r="E119" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F119" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>71</v>
       </c>
@@ -2784,8 +3156,11 @@
       <c r="E120" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F120" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>71</v>
       </c>
@@ -2801,8 +3176,11 @@
       <c r="E121" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F121" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>71</v>
       </c>
@@ -2818,8 +3196,11 @@
       <c r="E122" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F122" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>71</v>
       </c>
@@ -2835,8 +3216,11 @@
       <c r="E123" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F123" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>71</v>
       </c>
@@ -2852,8 +3236,11 @@
       <c r="E124" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F124" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>71</v>
       </c>
@@ -2869,8 +3256,11 @@
       <c r="E125" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F125" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>71</v>
       </c>
@@ -2886,8 +3276,11 @@
       <c r="E126" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F126" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="7" t="s">
         <v>71</v>
       </c>
@@ -2903,8 +3296,11 @@
       <c r="E127" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F127" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="7" t="s">
         <v>71</v>
       </c>
@@ -2920,8 +3316,11 @@
       <c r="E128" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F128" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>71</v>
       </c>
@@ -2937,8 +3336,11 @@
       <c r="E129" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F129" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>71</v>
       </c>
@@ -2954,8 +3356,11 @@
       <c r="E130" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F130" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="7" t="s">
         <v>71</v>
       </c>
@@ -2971,8 +3376,11 @@
       <c r="E131" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F131" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="7" t="s">
         <v>71</v>
       </c>
@@ -2988,8 +3396,11 @@
       <c r="E132" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F132" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="7" t="s">
         <v>71</v>
       </c>
@@ -3005,8 +3416,11 @@
       <c r="E133" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F133" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="7" t="s">
         <v>71</v>
       </c>
@@ -3022,8 +3436,11 @@
       <c r="E134" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F134" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="7" t="s">
         <v>71</v>
       </c>
@@ -3039,8 +3456,11 @@
       <c r="E135" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F135" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="7" t="s">
         <v>71</v>
       </c>
@@ -3056,8 +3476,11 @@
       <c r="E136" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F136" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="7" t="s">
         <v>71</v>
       </c>
@@ -3073,8 +3496,11 @@
       <c r="E137" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F137" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="7" t="s">
         <v>71</v>
       </c>
@@ -3090,8 +3516,11 @@
       <c r="E138" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F138" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="7" t="s">
         <v>71</v>
       </c>
@@ -3107,8 +3536,11 @@
       <c r="E139" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F139" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="7" t="s">
         <v>71</v>
       </c>
@@ -3124,8 +3556,11 @@
       <c r="E140" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F140" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
         <v>71</v>
       </c>
@@ -3141,8 +3576,11 @@
       <c r="E141" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F141" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="7" t="s">
         <v>71</v>
       </c>
@@ -3158,8 +3596,11 @@
       <c r="E142" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F142" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="7" t="s">
         <v>71</v>
       </c>
@@ -3175,8 +3616,11 @@
       <c r="E143" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F143" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="7" t="s">
         <v>71</v>
       </c>
@@ -3192,8 +3636,11 @@
       <c r="E144" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F144" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" s="7" t="s">
         <v>71</v>
       </c>
@@ -3209,8 +3656,11 @@
       <c r="E145" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F145" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="7" t="s">
         <v>71</v>
       </c>
@@ -3226,8 +3676,11 @@
       <c r="E146" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F146" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="7" t="s">
         <v>71</v>
       </c>
@@ -3243,8 +3696,11 @@
       <c r="E147" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F147" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="7" t="s">
         <v>71</v>
       </c>
@@ -3260,8 +3716,11 @@
       <c r="E148" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F148" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="7" t="s">
         <v>71</v>
       </c>
@@ -3277,8 +3736,11 @@
       <c r="E149" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F149" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="7" t="s">
         <v>71</v>
       </c>
@@ -3294,8 +3756,11 @@
       <c r="E150" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F150" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>13</v>
       </c>
@@ -3311,8 +3776,11 @@
       <c r="E151" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F151" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>13</v>
       </c>
@@ -3328,8 +3796,11 @@
       <c r="E152" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F152" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>1</v>
       </c>
@@ -3345,8 +3816,11 @@
       <c r="E153" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F153" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>71</v>
       </c>
@@ -3362,8 +3836,11 @@
       <c r="E154" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F154" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>71</v>
       </c>
@@ -3379,8 +3856,11 @@
       <c r="E155" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F155" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>1</v>
       </c>
@@ -3396,8 +3876,11 @@
       <c r="E156" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F156" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>1</v>
       </c>
@@ -3413,8 +3896,11 @@
       <c r="E157" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F157" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>71</v>
       </c>
@@ -3430,8 +3916,11 @@
       <c r="E158" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F158" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="7" t="s">
         <v>71</v>
       </c>
@@ -3447,8 +3936,11 @@
       <c r="E159" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F159" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>1</v>
       </c>
@@ -3464,8 +3956,11 @@
       <c r="E160" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F160" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>1</v>
       </c>
@@ -3481,8 +3976,11 @@
       <c r="E161" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F161" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>1</v>
       </c>
@@ -3498,8 +3996,11 @@
       <c r="E162" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F162" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>1</v>
       </c>
@@ -3515,8 +4016,11 @@
       <c r="E163" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F163" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>1</v>
       </c>
@@ -3532,8 +4036,11 @@
       <c r="E164" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F164" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>1</v>
       </c>
@@ -3549,8 +4056,11 @@
       <c r="E165" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F165" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>1</v>
       </c>
@@ -3566,8 +4076,11 @@
       <c r="E166" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F166" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>1</v>
       </c>
@@ -3583,8 +4096,11 @@
       <c r="E167" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F167" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>1</v>
       </c>
@@ -3600,8 +4116,11 @@
       <c r="E168" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F168" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>1</v>
       </c>
@@ -3617,8 +4136,11 @@
       <c r="E169" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F169" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>1</v>
       </c>
@@ -3634,8 +4156,11 @@
       <c r="E170" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F170" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>71</v>
       </c>
@@ -3651,8 +4176,11 @@
       <c r="E171" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F171" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>71</v>
       </c>
@@ -3668,8 +4196,11 @@
       <c r="E172" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F172" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>71</v>
       </c>
@@ -3685,8 +4216,11 @@
       <c r="E173" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F173" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>71</v>
       </c>
@@ -3702,8 +4236,11 @@
       <c r="E174" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F174" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="7" t="s">
         <v>71</v>
       </c>
@@ -3719,8 +4256,11 @@
       <c r="E175" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F175" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>71</v>
       </c>
@@ -3736,8 +4276,11 @@
       <c r="E176" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F176" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>1</v>
       </c>
@@ -3753,8 +4296,11 @@
       <c r="E177" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F177" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>1</v>
       </c>
@@ -3770,8 +4316,11 @@
       <c r="E178" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F178" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>1</v>
       </c>
@@ -3787,8 +4336,11 @@
       <c r="E179" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F179" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>1</v>
       </c>
@@ -3804,8 +4356,11 @@
       <c r="E180" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F180" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>1</v>
       </c>
@@ -3821,8 +4376,11 @@
       <c r="E181" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F181" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>1</v>
       </c>
@@ -3838,8 +4396,11 @@
       <c r="E182" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F182" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>1</v>
       </c>
@@ -3855,8 +4416,11 @@
       <c r="E183" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F183" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>1</v>
       </c>
@@ -3872,8 +4436,11 @@
       <c r="E184" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F184" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>1</v>
       </c>
@@ -3889,8 +4456,11 @@
       <c r="E185" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F185" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>1</v>
       </c>
@@ -3906,8 +4476,11 @@
       <c r="E186" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F186" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>1</v>
       </c>
@@ -3923,8 +4496,11 @@
       <c r="E187" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F187" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>1</v>
       </c>
@@ -3940,8 +4516,11 @@
       <c r="E188" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F188" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>1</v>
       </c>
@@ -3957,8 +4536,11 @@
       <c r="E189" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F189" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>1</v>
       </c>
@@ -3974,8 +4556,11 @@
       <c r="E190" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F190" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>1</v>
       </c>
@@ -3991,8 +4576,11 @@
       <c r="E191" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F191" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>1</v>
       </c>
@@ -4008,8 +4596,11 @@
       <c r="E192" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F192" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>1</v>
       </c>
@@ -4025,8 +4616,11 @@
       <c r="E193" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F193" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>1</v>
       </c>
@@ -4042,8 +4636,11 @@
       <c r="E194" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F194" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>1</v>
       </c>
@@ -4059,8 +4656,11 @@
       <c r="E195" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F195" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>1</v>
       </c>
@@ -4076,8 +4676,11 @@
       <c r="E196" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F196" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>1</v>
       </c>
@@ -4093,8 +4696,11 @@
       <c r="E197" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F197" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>1</v>
       </c>
@@ -4110,8 +4716,11 @@
       <c r="E198" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F198" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>1</v>
       </c>
@@ -4127,8 +4736,11 @@
       <c r="E199" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F199" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>1</v>
       </c>
@@ -4144,8 +4756,11 @@
       <c r="E200" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F200" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>1</v>
       </c>
@@ -4161,8 +4776,11 @@
       <c r="E201" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F201" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>1</v>
       </c>
@@ -4178,8 +4796,11 @@
       <c r="E202" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F202" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>1</v>
       </c>
@@ -4195,8 +4816,11 @@
       <c r="E203" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F203" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>1</v>
       </c>
@@ -4212,8 +4836,11 @@
       <c r="E204" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F204" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>1</v>
       </c>
@@ -4229,8 +4856,11 @@
       <c r="E205" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F205" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>1</v>
       </c>
@@ -4246,8 +4876,11 @@
       <c r="E206" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F206" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>1</v>
       </c>
@@ -4263,8 +4896,11 @@
       <c r="E207" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F207" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>1</v>
       </c>
@@ -4280,8 +4916,11 @@
       <c r="E208" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F208" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>1</v>
       </c>
@@ -4297,8 +4936,11 @@
       <c r="E209" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F209" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>1</v>
       </c>
@@ -4314,8 +4956,11 @@
       <c r="E210" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F210" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>1</v>
       </c>
@@ -4331,8 +4976,11 @@
       <c r="E211" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F211" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>1</v>
       </c>
@@ -4348,8 +4996,11 @@
       <c r="E212" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F212" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>1</v>
       </c>
@@ -4365,8 +5016,11 @@
       <c r="E213" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F213" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>1</v>
       </c>
@@ -4382,8 +5036,11 @@
       <c r="E214" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F214" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>1</v>
       </c>
@@ -4399,8 +5056,11 @@
       <c r="E215" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F215" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>1</v>
       </c>
@@ -4416,8 +5076,11 @@
       <c r="E216" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F216" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>1</v>
       </c>
@@ -4433,8 +5096,11 @@
       <c r="E217" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F217" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>1</v>
       </c>
@@ -4450,8 +5116,11 @@
       <c r="E218" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F218" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>1</v>
       </c>
@@ -4467,8 +5136,11 @@
       <c r="E219" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F219" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>13</v>
       </c>
@@ -4484,8 +5156,11 @@
       <c r="E220" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F220" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>13</v>
       </c>
@@ -4501,8 +5176,11 @@
       <c r="E221" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F221" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>1</v>
       </c>
@@ -4518,8 +5196,11 @@
       <c r="E222" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F222" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>1</v>
       </c>
@@ -4535,8 +5216,11 @@
       <c r="E223" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F223" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>1</v>
       </c>
@@ -4552,8 +5236,11 @@
       <c r="E224" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F224" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>13</v>
       </c>
@@ -4569,8 +5256,11 @@
       <c r="E225" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F225" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>1</v>
       </c>
@@ -4586,8 +5276,11 @@
       <c r="E226" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F226" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>1</v>
       </c>
@@ -4603,8 +5296,11 @@
       <c r="E227" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F227" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>1</v>
       </c>
@@ -4620,8 +5316,11 @@
       <c r="E228" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F228" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>1</v>
       </c>
@@ -4637,8 +5336,11 @@
       <c r="E229" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F229" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>1</v>
       </c>
@@ -4654,8 +5356,11 @@
       <c r="E230" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F230" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>1</v>
       </c>
@@ -4671,8 +5376,11 @@
       <c r="E231" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F231" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>1</v>
       </c>
@@ -4688,8 +5396,11 @@
       <c r="E232" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F232" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>1</v>
       </c>
@@ -4705,8 +5416,11 @@
       <c r="E233" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F233" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>1</v>
       </c>
@@ -4722,8 +5436,11 @@
       <c r="E234" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F234" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>1</v>
       </c>
@@ -4739,8 +5456,11 @@
       <c r="E235" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F235" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>1</v>
       </c>
@@ -4756,8 +5476,11 @@
       <c r="E236" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F236" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>1</v>
       </c>
@@ -4773,8 +5496,11 @@
       <c r="E237" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F237" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>1</v>
       </c>
@@ -4790,8 +5516,11 @@
       <c r="E238" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F238" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>1</v>
       </c>
@@ -4807,8 +5536,11 @@
       <c r="E239" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F239" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A240" s="7" t="s">
         <v>71</v>
       </c>
@@ -4824,8 +5556,11 @@
       <c r="E240" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F240" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>1</v>
       </c>
@@ -4841,8 +5576,11 @@
       <c r="E241" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F241" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>1</v>
       </c>
@@ -4858,8 +5596,11 @@
       <c r="E242" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F242" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>1</v>
       </c>
@@ -4875,8 +5616,11 @@
       <c r="E243" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F243" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
         <v>1</v>
       </c>
@@ -4892,13 +5636,11 @@
       <c r="E244" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="F244" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{7F217761-C46D-4553-9B08-6E524775D494}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E250">
-      <sortCondition ref="D1"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E251">
     <sortCondition ref="D2:D251"/>
     <sortCondition ref="B2:B251"/>

</xml_diff>